<commit_message>
feat: update api version and invoice template
</commit_message>
<xml_diff>
--- a/exports/invoice_template.xlsx
+++ b/exports/invoice_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dang.nguyenhai/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EB59F1-BB35-964E-B69E-DCB44DE9EE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBA1FE3-8E5D-ED4E-90D0-DD7BFAEEB2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16080" xr2:uid="{42B9C3C5-ADDF-2D47-A595-A92C02917BAE}"/>
   </bookViews>
@@ -361,18 +361,12 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -496,8 +490,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -505,12 +523,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -520,29 +532,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -864,7 +858,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -881,15 +875,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:22" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="B2" s="4"/>
@@ -903,16 +897,16 @@
       <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="G3" s="20" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="G3" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="20"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:22" s="5" customFormat="1" ht="14" customHeight="1">
       <c r="B4" s="10"/>
@@ -927,16 +921,16 @@
         <v>18</v>
       </c>
       <c r="B5" s="19"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="30" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="2" t="s">
         <v>22</v>
       </c>
@@ -947,47 +941,47 @@
         <v>19</v>
       </c>
       <c r="B6" s="19"/>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:22" ht="20" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="21" t="s">
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:22" ht="19" customHeight="1">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
       <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:22" s="5" customFormat="1" ht="19" customHeight="1">
@@ -1005,45 +999,45 @@
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="16" t="s">
+      <c r="C10" s="23"/>
+      <c r="D10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="29"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:22" ht="23" customHeight="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:22" ht="23" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="29"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="29"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="14" spans="1:22" ht="20" customHeight="1">
       <c r="A14" s="6" t="s">
@@ -1085,16 +1079,16 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" ht="19" customHeight="1">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1111,16 +1105,16 @@
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" ht="20" customHeight="1">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1137,52 +1131,52 @@
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" ht="17">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:22" ht="20" customHeight="1">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:22" ht="20" customHeight="1">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:22" ht="20" customHeight="1">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:22">
       <c r="B22" s="9" t="s">
@@ -1194,26 +1188,12 @@
       <c r="E23" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A20:H20"/>
     <mergeCell ref="A21:H21"/>
@@ -1225,6 +1205,20 @@
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A18:H18"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: update pending invoice update api
</commit_message>
<xml_diff>
--- a/exports/invoice_template.xlsx
+++ b/exports/invoice_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dang.nguyenhai/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBA1FE3-8E5D-ED4E-90D0-DD7BFAEEB2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE0D997-51E3-C343-9450-9E383743598A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16080" xr2:uid="{42B9C3C5-ADDF-2D47-A595-A92C02917BAE}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$40</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>グエン　カン　ズィ</t>
   </si>
@@ -87,10 +87,6 @@
   </si>
   <si>
     <t>2.提出された身分証明書が偽造・第三者のものであった場合は買取をお断り致します。</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>8.未成年の方からの商品の買取は（保護者の同意書がない限り）お断りしております。上記確認事項に同意しましたので、買取を依頼致します。</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -268,6 +264,12 @@
       <t>ニチ</t>
     </rPh>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>8.未成年の方からの商品の買取は（保護者の同意書がない限り）お断りしております。上記確認事項に同意しましたので、</t>
+  </si>
+  <si>
+    <t>買取を依頼致します。</t>
   </si>
 </sst>
 </file>
@@ -444,7 +446,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -472,9 +474,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -493,6 +492,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -502,7 +525,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -514,29 +540,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,10 +863,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -868,22 +876,22 @@
     <col min="3" max="3" width="23" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:22" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="B2" s="4"/>
@@ -891,157 +899,157 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1">
-      <c r="B3" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="G3" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="26"/>
+      <c r="B3" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="G3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:22" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:22" ht="23" customHeight="1">
       <c r="A5" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="19"/>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="29"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:22" ht="22" customHeight="1">
       <c r="A6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:22" ht="20" customHeight="1">
+      <c r="A7" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="1:22" ht="20" customHeight="1">
-      <c r="A7" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="12"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:22" ht="19" customHeight="1">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="12"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:22" s="5" customFormat="1" ht="19" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:22" ht="21" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="15" t="s">
+      <c r="G10" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:22" ht="23" customHeight="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:22" ht="23" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="17"/>
+      <c r="B12" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="14" spans="1:22" ht="20" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1079,16 +1087,16 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" ht="19" customHeight="1">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1105,16 +1113,16 @@
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" ht="20" customHeight="1">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1131,73 +1139,90 @@
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" ht="17">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="1:22" ht="20" customHeight="1">
+      <c r="A19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="1:22" ht="20" customHeight="1">
+      <c r="A20" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:22" ht="20" customHeight="1">
+      <c r="A21" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="19" customHeight="1">
+      <c r="B23" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-    </row>
-    <row r="19" spans="1:22" ht="20" customHeight="1">
-      <c r="A19" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-    </row>
-    <row r="20" spans="1:22" ht="20" customHeight="1">
-      <c r="A20" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-    </row>
-    <row r="21" spans="1:22" ht="20" customHeight="1">
-      <c r="A21" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-    </row>
-    <row r="22" spans="1:22">
-      <c r="B22" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" spans="1:22" ht="19" customHeight="1">
-      <c r="E23" s="7" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A20:H20"/>
     <mergeCell ref="A21:H21"/>
-    <mergeCell ref="F23:H23"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G7:H8"/>
@@ -1205,23 +1230,15 @@
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A18:H18"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G6:H6"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="72" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="79" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update excel template
</commit_message>
<xml_diff>
--- a/exports/invoice_template.xlsx
+++ b/exports/invoice_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dang.nguyenhai/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE0D997-51E3-C343-9450-9E383743598A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5AFB18-5607-2649-A322-253B64749553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16080" xr2:uid="{42B9C3C5-ADDF-2D47-A595-A92C02917BAE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>グエン　カン　ズィ</t>
   </si>
@@ -71,12 +71,6 @@
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>状態</t>
-  </si>
-  <si>
-    <t>単価</t>
   </si>
   <si>
     <t>署名:</t>
@@ -230,31 +224,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <r>
-      <t>東京都公安委員会許可　第</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 304372117441 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐ明朝"/>
-        <family val="1"/>
-        <charset val="128"/>
-      </rPr>
-      <t>号</t>
-    </r>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>東京都公安委員会許可　第 304372117441 号</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -270,6 +239,17 @@
   </si>
   <si>
     <t>買取を依頼致します。</t>
+  </si>
+  <si>
+    <t>色</t>
+    <rPh sb="0" eb="1">
+      <t>イロ</t>
+    </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>状態</t>
+    <phoneticPr fontId="12"/>
   </si>
 </sst>
 </file>
@@ -363,12 +343,18 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -498,13 +484,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -514,36 +530,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -863,10 +849,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -883,38 +869,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30">
-      <c r="B1" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="B1" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:22" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="F2" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1">
-      <c r="B3" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="G3" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="20"/>
+      <c r="B3" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="G3" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:22" s="5" customFormat="1" ht="14" customHeight="1">
       <c r="B4" s="9"/>
@@ -925,71 +911,71 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:22" ht="23" customHeight="1">
-      <c r="A5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="19"/>
+      <c r="A5" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="27"/>
       <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="31"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:22" ht="22" customHeight="1">
-      <c r="A6" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="19"/>
+      <c r="A6" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="27"/>
       <c r="C6" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="19"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:22" ht="20" customHeight="1">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="21"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="31"/>
       <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:22" ht="19" customHeight="1">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:22" s="5" customFormat="1" ht="19" customHeight="1">
@@ -1007,49 +993,49 @@
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="24"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:22" ht="23" customHeight="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:22" ht="23" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="24"/>
+      <c r="B12" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="14" spans="1:22" ht="20" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1062,7 +1048,7 @@
     </row>
     <row r="15" spans="1:22" ht="20" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1087,16 +1073,16 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" ht="19" customHeight="1">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1113,16 +1099,16 @@
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" ht="20" customHeight="1">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1139,79 +1125,82 @@
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" ht="17">
-      <c r="A18" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
+      <c r="A18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:22" ht="20" customHeight="1">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
     </row>
     <row r="20" spans="1:22" ht="20" customHeight="1">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:22" ht="20" customHeight="1">
-      <c r="A21" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
+      <c r="A21" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="19" customHeight="1">
-      <c r="B23" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:22">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
+      <c r="E24" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B23:D23"/>
+  <mergeCells count="26">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A5:B5"/>
@@ -1220,22 +1209,24 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A21:H21"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G7:H8"/>
     <mergeCell ref="C7:F8"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:H25"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:H21"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: update excel template new
</commit_message>
<xml_diff>
--- a/exports/invoice_template.xlsx
+++ b/exports/invoice_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dang.nguyenhai/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A727C7CC-E8D2-BA4D-8AB2-5C2C48A78FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EA2859-DB3A-8440-B8CE-86066CFBA55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="500" windowWidth="28300" windowHeight="16080" xr2:uid="{42B9C3C5-ADDF-2D47-A595-A92C02917BAE}"/>
   </bookViews>
@@ -493,6 +493,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -516,24 +534,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,8 +854,8 @@
   </sheetPr>
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -872,38 +872,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:22" s="5" customFormat="1" ht="17" customHeight="1">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="G3" s="25" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="G3" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="25"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:22" s="5" customFormat="1" ht="14" customHeight="1">
       <c r="B4" s="9"/>
@@ -914,71 +914,71 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:22" ht="23" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:22" ht="22" customHeight="1">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="22"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="30"/>
+      <c r="G6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:22" ht="20" customHeight="1">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="27" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="26" t="s">
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="32"/>
       <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:22" ht="19" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
       <c r="I8" s="11"/>
     </row>
     <row r="9" spans="1:22" s="5" customFormat="1" ht="19" customHeight="1">
@@ -996,10 +996,10 @@
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="31"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="18" t="s">
         <v>31</v>
       </c>
@@ -1009,32 +1009,32 @@
       <c r="F10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="29"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:22" ht="23" customHeight="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:22" ht="23" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="29"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="29"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="23"/>
     </row>
     <row r="14" spans="1:22" ht="20" customHeight="1">
       <c r="A14" s="6" t="s">
@@ -1076,16 +1076,16 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" ht="19" customHeight="1">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1102,16 +1102,16 @@
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" ht="20" customHeight="1">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1128,52 +1128,52 @@
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" ht="17">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:22" ht="20" customHeight="1">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
     </row>
     <row r="20" spans="1:22" ht="20" customHeight="1">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:22" ht="20" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="5" t="s">
@@ -1185,16 +1185,16 @@
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
     </row>
-    <row r="24" spans="1:22" ht="42" customHeight="1">
+    <row r="24" spans="1:22" ht="46" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="29"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="23"/>
     </row>
     <row r="25" spans="1:22">
       <c r="E25" s="5"/>
@@ -1204,19 +1204,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A5:B5"/>
@@ -1229,6 +1216,19 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G7:H8"/>
     <mergeCell ref="C7:F8"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>